<commit_message>
Add produce Logic of SLG Building
</commit_message>
<xml_diff>
--- a/_Out/Server/NFDataCfg/Excel_Struct/BB_Build.xlsx
+++ b/_Out/Server/NFDataCfg/Excel_Struct/BB_Build.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\work\NoahGameFrame\_Out\Server\NFDataCfg\Excel_Struct\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\NF\NoahGameFrame\_Out\Server\NFDataCfg\Excel_Struct\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="25">
   <si>
     <t>Id</t>
   </si>
@@ -51,66 +51,59 @@
     <t>Desc</t>
   </si>
   <si>
+    <t>Friend</t>
+  </si>
+  <si>
+    <t>int</t>
+  </si>
+  <si>
+    <t>Type</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SubType</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Prefab</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NormalStateFunc</t>
+  </si>
+  <si>
+    <t>UpStateFunc</t>
+  </si>
+  <si>
+    <t>Desc</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>建筑类型</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>建筑子类型</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>预设路径</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>普通状态下函数</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>升级状态函数</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>描述</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>string</t>
-  </si>
-  <si>
-    <t>Friend</t>
-  </si>
-  <si>
-    <t>int</t>
-  </si>
-  <si>
-    <t>ID</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Type</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SubType</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Prefab</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>NormalStateFunc</t>
-  </si>
-  <si>
-    <t>UpStateFunc</t>
-  </si>
-  <si>
-    <t>Desc</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>建筑ID</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>建筑类型</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>建筑子类型</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>预设路径</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>普通状态下函数</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>升级状态函数</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>描述</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -508,10 +501,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J8"/>
+  <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -561,42 +554,42 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F2" t="b">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C2" t="b">
-        <v>0</v>
-      </c>
-      <c r="D2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F2" t="b">
-        <v>0</v>
-      </c>
-      <c r="G2">
-        <v>0</v>
-      </c>
-      <c r="H2">
-        <v>0</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>11</v>
-      </c>
       <c r="J2" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C3" t="b">
         <v>0</v>
@@ -617,18 +610,18 @@
         <v>0</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="C4" t="b">
         <v>0</v>
@@ -649,18 +642,18 @@
         <v>0</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A5" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="C5" t="b">
         <v>0</v>
@@ -681,18 +674,18 @@
         <v>0</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="C6" t="b">
         <v>0</v>
@@ -713,18 +706,18 @@
         <v>0</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A7" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="C7" t="b">
         <v>0</v>
@@ -745,49 +738,17 @@
         <v>0</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A8" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C8" t="b">
-        <v>0</v>
-      </c>
-      <c r="D8" t="b">
-        <v>0</v>
-      </c>
-      <c r="E8" t="b">
-        <v>0</v>
-      </c>
-      <c r="F8" t="b">
-        <v>0</v>
-      </c>
-      <c r="G8">
-        <v>0</v>
-      </c>
-      <c r="H8">
-        <v>0</v>
-      </c>
-      <c r="I8" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="J8" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <dataValidations disablePrompts="1" count="2">
+  <dataValidations count="2">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F1"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F9:F1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F8:F1048576">
       <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>